<commit_message>
fix div tagas facing
</commit_message>
<xml_diff>
--- a/media/PM_Report_16.xlsx
+++ b/media/PM_Report_16.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -287,14 +287,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -304,33 +317,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -722,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -738,171 +738,171 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="E1" s="18" t="inlineStr">
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>ANNEX "E"</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1">
-      <c r="A3" s="13" t="inlineStr">
+      <c r="A3" s="18" t="inlineStr">
         <is>
           <t>Preventive Maintenance Checklist/Activities</t>
         </is>
       </c>
-      <c r="F3" s="12" t="n"/>
-      <c r="G3" s="12" t="n"/>
-      <c r="H3" s="12" t="n"/>
-      <c r="I3" s="12" t="n"/>
-      <c r="J3" s="12" t="n"/>
-      <c r="K3" s="12" t="n"/>
+      <c r="F3" s="17" t="n"/>
+      <c r="G3" s="17" t="n"/>
+      <c r="H3" s="17" t="n"/>
+      <c r="I3" s="17" t="n"/>
+      <c r="J3" s="17" t="n"/>
+      <c r="K3" s="17" t="n"/>
     </row>
     <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="13" t="inlineStr">
+      <c r="A4" s="18" t="inlineStr">
         <is>
           <t>For Workstation (Quarterly)</t>
         </is>
       </c>
-      <c r="F4" s="12" t="n"/>
-      <c r="G4" s="12" t="n"/>
-      <c r="H4" s="12" t="n"/>
-      <c r="I4" s="12" t="n"/>
-      <c r="J4" s="12" t="n"/>
-      <c r="K4" s="12" t="n"/>
+      <c r="F4" s="17" t="n"/>
+      <c r="G4" s="17" t="n"/>
+      <c r="H4" s="17" t="n"/>
+      <c r="I4" s="17" t="n"/>
+      <c r="J4" s="17" t="n"/>
+      <c r="K4" s="17" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n"/>
-      <c r="B5" s="11" t="n"/>
-      <c r="C5" s="11" t="n"/>
-      <c r="D5" s="11" t="n"/>
-      <c r="E5" s="11" t="n"/>
-      <c r="F5" s="11" t="n"/>
-      <c r="G5" s="11" t="n"/>
-      <c r="H5" s="11" t="n"/>
-      <c r="I5" s="11" t="n"/>
-      <c r="J5" s="11" t="n"/>
-      <c r="K5" s="11" t="n"/>
+      <c r="A5" s="16" t="n"/>
+      <c r="B5" s="16" t="n"/>
+      <c r="C5" s="16" t="n"/>
+      <c r="D5" s="16" t="n"/>
+      <c r="E5" s="16" t="n"/>
+      <c r="F5" s="16" t="n"/>
+      <c r="G5" s="16" t="n"/>
+      <c r="H5" s="16" t="n"/>
+      <c r="I5" s="16" t="n"/>
+      <c r="J5" s="16" t="n"/>
+      <c r="K5" s="16" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="17" t="inlineStr">
         <is>
           <t>Schedule: As approved by head Office</t>
         </is>
       </c>
-      <c r="B6" s="11" t="n"/>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
-      <c r="E6" s="11" t="n"/>
-      <c r="F6" s="11" t="n"/>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="11" t="n"/>
-      <c r="I6" s="11" t="n"/>
-      <c r="J6" s="11" t="n"/>
-      <c r="K6" s="11" t="n"/>
+      <c r="B6" s="16" t="n"/>
+      <c r="C6" s="16" t="n"/>
+      <c r="D6" s="16" t="n"/>
+      <c r="E6" s="16" t="n"/>
+      <c r="F6" s="16" t="n"/>
+      <c r="G6" s="16" t="n"/>
+      <c r="H6" s="16" t="n"/>
+      <c r="I6" s="16" t="n"/>
+      <c r="J6" s="16" t="n"/>
+      <c r="K6" s="16" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="17" t="inlineStr">
         <is>
           <t>Office:</t>
         </is>
       </c>
-      <c r="B7" s="11" t="n"/>
-      <c r="C7" s="11" t="inlineStr">
+      <c r="B7" s="16" t="n"/>
+      <c r="C7" s="16" t="inlineStr">
         <is>
           <t>Finance Section</t>
         </is>
       </c>
-      <c r="E7" s="11" t="n"/>
-      <c r="F7" s="11" t="n"/>
-      <c r="G7" s="11" t="n"/>
-      <c r="H7" s="11" t="n"/>
-      <c r="I7" s="11" t="n"/>
-      <c r="J7" s="11" t="n"/>
-      <c r="K7" s="11" t="n"/>
+      <c r="E7" s="16" t="n"/>
+      <c r="F7" s="16" t="n"/>
+      <c r="G7" s="16" t="n"/>
+      <c r="H7" s="16" t="n"/>
+      <c r="I7" s="16" t="n"/>
+      <c r="J7" s="16" t="n"/>
+      <c r="K7" s="16" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="inlineStr">
+      <c r="A8" s="19" t="inlineStr">
         <is>
           <t>Computer Name:</t>
         </is>
       </c>
-      <c r="C8" s="12" t="inlineStr">
-        <is>
-          <t>rr33x</t>
-        </is>
-      </c>
-      <c r="E8" s="11" t="n"/>
-      <c r="F8" s="11" t="n"/>
-      <c r="G8" s="11" t="n"/>
-      <c r="H8" s="11" t="n"/>
-      <c r="I8" s="11" t="n"/>
-      <c r="J8" s="11" t="n"/>
-      <c r="K8" s="11" t="n"/>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>R08-LEY4-048</t>
+        </is>
+      </c>
+      <c r="E8" s="16" t="n"/>
+      <c r="F8" s="16" t="n"/>
+      <c r="G8" s="16" t="n"/>
+      <c r="H8" s="16" t="n"/>
+      <c r="I8" s="16" t="n"/>
+      <c r="J8" s="16" t="n"/>
+      <c r="K8" s="16" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="inlineStr">
+      <c r="A9" s="19" t="inlineStr">
         <is>
           <t>End user:</t>
         </is>
       </c>
-      <c r="C9" s="12" t="inlineStr">
+      <c r="C9" s="17" t="inlineStr">
         <is>
           <t>Lazarus Zacharias</t>
         </is>
       </c>
-      <c r="E9" s="11" t="n"/>
-      <c r="F9" s="11" t="n"/>
-      <c r="G9" s="11" t="n"/>
-      <c r="H9" s="11" t="n"/>
-      <c r="I9" s="11" t="n"/>
-      <c r="J9" s="11" t="n"/>
-      <c r="K9" s="11" t="n"/>
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="16" t="n"/>
+      <c r="G9" s="16" t="n"/>
+      <c r="H9" s="16" t="n"/>
+      <c r="I9" s="16" t="n"/>
+      <c r="J9" s="16" t="n"/>
+      <c r="K9" s="16" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="inlineStr">
+      <c r="A10" s="17" t="inlineStr">
         <is>
           <t>Date accomplished:</t>
         </is>
       </c>
-      <c r="B10" s="11" t="n"/>
-      <c r="C10" s="11" t="inlineStr">
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="16" t="inlineStr">
         <is>
           <t>2025-10-17</t>
         </is>
       </c>
-      <c r="E10" s="11" t="n"/>
-      <c r="F10" s="11" t="n"/>
-      <c r="G10" s="11" t="n"/>
-      <c r="H10" s="11" t="n"/>
-      <c r="I10" s="11" t="n"/>
-      <c r="J10" s="11" t="n"/>
-      <c r="K10" s="11" t="n"/>
+      <c r="E10" s="16" t="n"/>
+      <c r="F10" s="16" t="n"/>
+      <c r="G10" s="16" t="n"/>
+      <c r="H10" s="16" t="n"/>
+      <c r="I10" s="16" t="n"/>
+      <c r="J10" s="16" t="n"/>
+      <c r="K10" s="16" t="n"/>
     </row>
     <row r="11" ht="3.75" customHeight="1">
-      <c r="A11" s="12" t="n"/>
-      <c r="B11" s="11" t="n"/>
-      <c r="C11" s="11" t="n"/>
-      <c r="D11" s="11" t="n"/>
-      <c r="E11" s="11" t="n"/>
-      <c r="F11" s="11" t="n"/>
-      <c r="G11" s="11" t="n"/>
-      <c r="H11" s="11" t="n"/>
-      <c r="I11" s="11" t="n"/>
-      <c r="J11" s="11" t="n"/>
-      <c r="K11" s="11" t="n"/>
+      <c r="A11" s="17" t="n"/>
+      <c r="B11" s="16" t="n"/>
+      <c r="C11" s="16" t="n"/>
+      <c r="D11" s="16" t="n"/>
+      <c r="E11" s="16" t="n"/>
+      <c r="F11" s="16" t="n"/>
+      <c r="G11" s="16" t="n"/>
+      <c r="H11" s="16" t="n"/>
+      <c r="I11" s="16" t="n"/>
+      <c r="J11" s="16" t="n"/>
+      <c r="K11" s="16" t="n"/>
     </row>
     <row r="12" ht="7.5" customHeight="1">
-      <c r="A12" s="11" t="n"/>
-      <c r="B12" s="11" t="n"/>
-      <c r="C12" s="11" t="n"/>
-      <c r="D12" s="11" t="n"/>
-      <c r="E12" s="11" t="n"/>
-      <c r="F12" s="11" t="n"/>
-      <c r="G12" s="11" t="n"/>
-      <c r="H12" s="11" t="n"/>
-      <c r="I12" s="11" t="n"/>
-      <c r="J12" s="11" t="n"/>
-      <c r="K12" s="11" t="n"/>
+      <c r="A12" s="16" t="n"/>
+      <c r="B12" s="16" t="n"/>
+      <c r="C12" s="16" t="n"/>
+      <c r="D12" s="16" t="n"/>
+      <c r="E12" s="16" t="n"/>
+      <c r="F12" s="16" t="n"/>
+      <c r="G12" s="16" t="n"/>
+      <c r="H12" s="16" t="n"/>
+      <c r="I12" s="16" t="n"/>
+      <c r="J12" s="16" t="n"/>
+      <c r="K12" s="16" t="n"/>
     </row>
     <row r="13" ht="41.25" customHeight="1" thickBot="1">
       <c r="A13" s="6" t="inlineStr">
@@ -926,11 +926,11 @@
           <t>Problems Encountered/ Action</t>
         </is>
       </c>
-      <c r="G13" s="11" t="n"/>
-      <c r="H13" s="11" t="n"/>
-      <c r="I13" s="11" t="n"/>
-      <c r="J13" s="11" t="n"/>
-      <c r="K13" s="11" t="n"/>
+      <c r="G13" s="16" t="n"/>
+      <c r="H13" s="16" t="n"/>
+      <c r="I13" s="16" t="n"/>
+      <c r="J13" s="16" t="n"/>
+      <c r="K13" s="16" t="n"/>
     </row>
     <row r="14" ht="53.25" customHeight="1">
       <c r="A14" s="5" t="n">
@@ -942,18 +942,22 @@
         </is>
       </c>
       <c r="C14" s="27" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E14" s="22" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="F14" s="11" t="n"/>
-      <c r="G14" s="11" t="n"/>
-      <c r="H14" s="11" t="n"/>
-      <c r="I14" s="11" t="n"/>
-      <c r="J14" s="11" t="n"/>
-      <c r="K14" s="11" t="n"/>
+      <c r="F14" s="16" t="n"/>
+      <c r="G14" s="16" t="n"/>
+      <c r="H14" s="16" t="n"/>
+      <c r="I14" s="16" t="n"/>
+      <c r="J14" s="16" t="n"/>
+      <c r="K14" s="16" t="n"/>
     </row>
     <row r="15" ht="39" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -965,14 +969,14 @@
         </is>
       </c>
       <c r="C15" s="29" t="n"/>
-      <c r="D15" s="3" t="n"/>
-      <c r="E15" s="9" t="inlineStr"/>
-      <c r="F15" s="11" t="n"/>
-      <c r="G15" s="11" t="n"/>
-      <c r="H15" s="11" t="n"/>
-      <c r="I15" s="11" t="n"/>
-      <c r="J15" s="11" t="n"/>
-      <c r="K15" s="11" t="n"/>
+      <c r="D15" s="3" t="inlineStr"/>
+      <c r="E15" s="23" t="inlineStr"/>
+      <c r="F15" s="16" t="n"/>
+      <c r="G15" s="16" t="n"/>
+      <c r="H15" s="16" t="n"/>
+      <c r="I15" s="16" t="n"/>
+      <c r="J15" s="16" t="n"/>
+      <c r="K15" s="16" t="n"/>
     </row>
     <row r="16" ht="51" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -986,18 +990,22 @@
         </is>
       </c>
       <c r="C16" s="29" t="n"/>
-      <c r="D16" s="3" t="n"/>
-      <c r="E16" s="9" t="inlineStr">
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E16" s="23" t="inlineStr">
         <is>
           <t>test3</t>
         </is>
       </c>
-      <c r="F16" s="11" t="n"/>
-      <c r="G16" s="11" t="n"/>
-      <c r="H16" s="11" t="n"/>
-      <c r="I16" s="11" t="n"/>
-      <c r="J16" s="11" t="n"/>
-      <c r="K16" s="11" t="n"/>
+      <c r="F16" s="16" t="n"/>
+      <c r="G16" s="16" t="n"/>
+      <c r="H16" s="16" t="n"/>
+      <c r="I16" s="16" t="n"/>
+      <c r="J16" s="16" t="n"/>
+      <c r="K16" s="16" t="n"/>
     </row>
     <row r="17" ht="48" customHeight="1">
       <c r="A17" s="4" t="n">
@@ -1010,8 +1018,12 @@
         </is>
       </c>
       <c r="C17" s="29" t="n"/>
-      <c r="D17" s="4" t="n"/>
-      <c r="E17" s="10" t="inlineStr">
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E17" s="24" t="inlineStr">
         <is>
           <t>testste 4</t>
         </is>
@@ -1029,8 +1041,12 @@
         </is>
       </c>
       <c r="C18" s="29" t="n"/>
-      <c r="D18" s="4" t="n"/>
-      <c r="E18" s="10" t="inlineStr">
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E18" s="24" t="inlineStr">
         <is>
           <t>test5</t>
         </is>
@@ -1050,8 +1066,12 @@
         </is>
       </c>
       <c r="C19" s="29" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="10" t="inlineStr">
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E19" s="24" t="inlineStr">
         <is>
           <t>testsetst 6</t>
         </is>
@@ -1068,8 +1088,12 @@
         </is>
       </c>
       <c r="C20" s="29" t="n"/>
-      <c r="D20" s="4" t="n"/>
-      <c r="E20" s="10" t="inlineStr">
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E20" s="24" t="inlineStr">
         <is>
           <t>testttst7</t>
         </is>
@@ -1087,8 +1111,12 @@
         </is>
       </c>
       <c r="C21" s="29" t="n"/>
-      <c r="D21" s="4" t="n"/>
-      <c r="E21" s="10" t="inlineStr">
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E21" s="24" t="inlineStr">
         <is>
           <t>testset 8</t>
         </is>
@@ -1106,8 +1134,12 @@
         </is>
       </c>
       <c r="C22" s="29" t="n"/>
-      <c r="D22" s="4" t="n"/>
-      <c r="E22" s="10" t="inlineStr">
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="E22" s="24" t="inlineStr">
         <is>
           <t>teststs 9</t>
         </is>
@@ -1116,24 +1148,24 @@
     <row r="23" ht="6" customHeight="1"/>
     <row r="24" ht="8.25" customHeight="1"/>
     <row r="25">
-      <c r="A25" s="17" t="inlineStr">
+      <c r="A25" s="8" t="inlineStr">
         <is>
           <t>Accomplished by:</t>
         </is>
       </c>
-      <c r="B25" s="17" t="n"/>
+      <c r="B25" s="8" t="n"/>
     </row>
     <row r="26" ht="22.5" customHeight="1">
-      <c r="A26" s="17" t="n"/>
-      <c r="B26" s="17" t="n"/>
+      <c r="A26" s="8" t="n"/>
+      <c r="B26" s="8" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="19" t="n"/>
+      <c r="A27" s="10" t="n"/>
       <c r="B27" s="30" t="n"/>
       <c r="C27" s="30" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="20" t="inlineStr">
+      <c r="A28" s="11" t="inlineStr">
         <is>
           <t>(Signature over printed name)</t>
         </is>

</xml_diff>